<commit_message>
Atualização LaTeX - Leonardo
</commit_message>
<xml_diff>
--- a/STB32/Confiabilidade.xlsx
+++ b/STB32/Confiabilidade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Confiabilidade\STB32\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projetos\Confiabilidade\STB32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728B2DC8-191E-43CA-9907-F07CC9FE8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9557B0B8-3935-438A-80E1-F28FF6F88895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="662" activeTab="4" xr2:uid="{BF70868E-A8BD-433C-AC44-EAE67A23BC06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="662" activeTab="4" xr2:uid="{BF70868E-A8BD-433C-AC44-EAE67A23BC06}"/>
   </bookViews>
   <sheets>
     <sheet name="Barras" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="SegmentaçãodeDados_Barra_PARA">#N/A</definedName>
     <definedName name="SegmentaçãodeDados_Circuito">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -44,7 +44,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -611,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -666,6 +668,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -25348,7 +25354,7 @@
       <c r="C2" s="1">
         <v>9.6</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="28" t="s">
         <v>98</v>
       </c>
       <c r="E2" s="1">
@@ -25366,7 +25372,7 @@
       <c r="I2" s="1">
         <v>897</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="29" t="s">
         <v>98</v>
       </c>
       <c r="L2" s="8">
@@ -25401,7 +25407,7 @@
       <c r="C3" s="1">
         <v>5.5</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="1">
         <v>13</v>
       </c>
@@ -25417,7 +25423,7 @@
       <c r="I3" s="1">
         <v>959</v>
       </c>
-      <c r="K3" s="27"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="8">
         <v>517</v>
       </c>
@@ -25450,7 +25456,7 @@
       <c r="C4" s="1">
         <v>5.2</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="1">
         <v>24</v>
       </c>
@@ -25466,7 +25472,7 @@
       <c r="I4" s="1">
         <v>979</v>
       </c>
-      <c r="K4" s="27"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="8">
         <v>508</v>
       </c>
@@ -25499,7 +25505,7 @@
       <c r="C5" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="1">
         <v>20</v>
       </c>
@@ -25515,7 +25521,7 @@
       <c r="I5" s="1">
         <v>976</v>
       </c>
-      <c r="K5" s="27"/>
+      <c r="K5" s="29"/>
       <c r="L5" s="8">
         <v>352</v>
       </c>
@@ -25548,7 +25554,7 @@
       <c r="C6" s="1">
         <v>3.5</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="1">
         <v>23</v>
       </c>
@@ -25564,7 +25570,7 @@
       <c r="I6" s="1">
         <v>964</v>
       </c>
-      <c r="K6" s="27"/>
+      <c r="K6" s="29"/>
       <c r="L6" s="8">
         <v>349</v>
       </c>
@@ -25609,7 +25615,7 @@
       <c r="I7" s="1">
         <v>979</v>
       </c>
-      <c r="K7" s="27"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="8">
         <v>487</v>
       </c>
@@ -25642,7 +25648,7 @@
       <c r="C8" s="1">
         <v>3.2</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="8">
         <v>528</v>
       </c>
@@ -25675,7 +25681,7 @@
       <c r="C9" s="1">
         <v>2.6</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="K9" s="29"/>
       <c r="L9" s="8">
         <v>449</v>
       </c>
@@ -25738,7 +25744,7 @@
       <c r="C10" s="1">
         <v>2.4</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="K10" s="29"/>
       <c r="L10" s="8">
         <v>470</v>
       </c>
@@ -25771,7 +25777,7 @@
       <c r="C11" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="29"/>
       <c r="L11" s="8">
         <v>538</v>
       </c>
@@ -25804,7 +25810,7 @@
       <c r="C12" s="1">
         <v>1.2</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="29"/>
       <c r="L12" s="8">
         <v>507</v>
       </c>
@@ -25837,7 +25843,7 @@
       <c r="C13" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K13" s="27"/>
+      <c r="K13" s="29"/>
       <c r="L13" s="8">
         <v>297</v>
       </c>
@@ -25870,7 +25876,7 @@
       <c r="C14" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K14" s="27"/>
+      <c r="K14" s="29"/>
       <c r="L14" s="8">
         <v>476</v>
       </c>
@@ -25903,7 +25909,7 @@
       <c r="C15" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="8">
         <v>269</v>
       </c>
@@ -25936,7 +25942,7 @@
       <c r="C16" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K16" s="27"/>
+      <c r="K16" s="29"/>
       <c r="L16" s="8">
         <v>448</v>
       </c>
@@ -25969,7 +25975,7 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="K17" s="27"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="8">
         <v>542</v>
       </c>
@@ -25993,7 +25999,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K18" s="27"/>
+      <c r="K18" s="29"/>
       <c r="L18" s="8">
         <v>539</v>
       </c>
@@ -26017,7 +26023,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K19" s="27"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="8">
         <v>272</v>
       </c>
@@ -26041,7 +26047,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K20" s="27"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="8">
         <v>541</v>
       </c>
@@ -26065,7 +26071,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K21" s="27"/>
+      <c r="K21" s="29"/>
       <c r="L21" s="8">
         <v>353</v>
       </c>
@@ -26089,7 +26095,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K22" s="27"/>
+      <c r="K22" s="29"/>
       <c r="L22" s="8">
         <v>468</v>
       </c>
@@ -26113,7 +26119,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K23" s="27" t="s">
+      <c r="K23" s="29" t="s">
         <v>104</v>
       </c>
       <c r="L23" s="8">
@@ -26135,7 +26141,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="27"/>
+      <c r="K24" s="29"/>
       <c r="L24" s="8">
         <v>529</v>
       </c>
@@ -26155,7 +26161,7 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K25" s="27"/>
+      <c r="K25" s="29"/>
       <c r="L25" s="8">
         <v>467</v>
       </c>
@@ -26175,7 +26181,7 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K26" s="27"/>
+      <c r="K26" s="29"/>
       <c r="L26" s="8">
         <v>446</v>
       </c>
@@ -26195,7 +26201,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K27" s="27"/>
+      <c r="K27" s="29"/>
       <c r="L27" s="8">
         <v>444</v>
       </c>
@@ -26215,7 +26221,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K28" s="27"/>
+      <c r="K28" s="29"/>
       <c r="L28" s="8">
         <v>377</v>
       </c>
@@ -26235,7 +26241,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K29" s="27"/>
+      <c r="K29" s="29"/>
       <c r="L29" s="8">
         <v>375</v>
       </c>
@@ -26255,7 +26261,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K30" s="27"/>
+      <c r="K30" s="29"/>
       <c r="L30" s="8">
         <v>326</v>
       </c>
@@ -26275,7 +26281,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K31" s="27"/>
+      <c r="K31" s="29"/>
       <c r="L31" s="8">
         <v>324</v>
       </c>
@@ -26295,7 +26301,7 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="27"/>
+      <c r="K32" s="29"/>
       <c r="L32" s="8">
         <v>320</v>
       </c>
@@ -26359,10 +26365,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA4C73E-833A-4410-9019-FF849DCE3D9B}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26377,9 +26383,10 @@
     <col min="8" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>38</v>
       </c>
@@ -26411,8 +26418,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="17">
@@ -26451,9 +26458,13 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>896-897</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="M2" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>3.0980999999999999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
       <c r="B3" s="17">
         <v>13</v>
       </c>
@@ -26490,9 +26501,13 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>938-959</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="M3" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>6.7836999999999997E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
       <c r="B4" s="17">
         <v>24</v>
       </c>
@@ -26529,9 +26544,13 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>995-979</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="M4" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>1.5422000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
       <c r="B5" s="17">
         <v>20</v>
       </c>
@@ -26568,9 +26587,13 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>964-976</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="M5" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>3.8747E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
       <c r="B6" s="17">
         <v>23</v>
       </c>
@@ -26607,8 +26630,12 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>995-964</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>1.2528000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>106</v>
       </c>
@@ -26646,8 +26673,12 @@
         <f>Tabela6[[#This Row],[De1]]&amp;"-"&amp;Tabela6[[#This Row],[Para1]]</f>
         <v>955-979</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="27">
+        <f>Tabela6[[#This Row],[Q]]</f>
+        <v>1.2646000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
@@ -26667,7 +26698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H10" s="24" t="s">
         <v>107</v>
       </c>
@@ -26680,7 +26711,7 @@
         <v>0.9945472624124081</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H11" s="24" t="s">
         <v>108</v>
       </c>
@@ -26693,13 +26724,13 @@
         <v>5.4527375875919049E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K14" s="3"/>
     </row>
   </sheetData>
@@ -26717,10 +26748,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7244C713-9829-49D0-8F24-8024894247D5}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="R32" sqref="R2:S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26741,10 +26772,12 @@
     <col min="14" max="14" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="17" max="19" width="9" style="1"/>
+    <col min="20" max="20" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
@@ -26794,8 +26827,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="8">
@@ -26852,9 +26885,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="R2" s="1" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="S2" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>960-1015</v>
+      </c>
+      <c r="T2" s="1">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3305622500000001E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="8">
         <v>517</v>
       </c>
@@ -26909,9 +26954,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="R3" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="S3" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1010-947</v>
+      </c>
+      <c r="T3" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3305622500000001E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
       <c r="B4" s="8">
         <v>508</v>
       </c>
@@ -26966,9 +27023,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="R4" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="S4" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>959-895</v>
+      </c>
+      <c r="T4" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3305622500000001E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
       <c r="B5" s="8">
         <v>352</v>
       </c>
@@ -27023,9 +27092,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="R5" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-955</v>
+      </c>
+      <c r="S5" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T5" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>7.5078759039999993E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
       <c r="B6" s="8">
         <v>349</v>
       </c>
@@ -27080,9 +27161,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="R6" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-955</v>
+      </c>
+      <c r="S6" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>938-946</v>
+      </c>
+      <c r="T6" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>7.5078759039999993E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
       <c r="B7" s="8">
         <v>487</v>
       </c>
@@ -27137,9 +27230,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="R7" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>947-939</v>
+      </c>
+      <c r="S7" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T7" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.1307078760000001E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
       <c r="B8" s="8">
         <v>528</v>
       </c>
@@ -27194,9 +27299,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="R8" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S8" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>965-1057</v>
+      </c>
+      <c r="T8" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
       <c r="B9" s="8">
         <v>449</v>
       </c>
@@ -27251,9 +27368,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
+      <c r="R9" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-946</v>
+      </c>
+      <c r="S9" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>960-1015</v>
+      </c>
+      <c r="T9" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.8299572840000001E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
       <c r="B10" s="8">
         <v>470</v>
       </c>
@@ -27308,9 +27437,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="R10" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="S10" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>960-1015</v>
+      </c>
+      <c r="T10" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5388402500000001E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
       <c r="B11" s="8">
         <v>538</v>
       </c>
@@ -27365,9 +27506,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="R11" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S11" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1047-1069</v>
+      </c>
+      <c r="T11" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
       <c r="B12" s="8">
         <v>507</v>
       </c>
@@ -27422,9 +27575,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="R12" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="S12" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="T12" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3305622500000001E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
       <c r="B13" s="8">
         <v>297</v>
       </c>
@@ -27479,9 +27644,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="R13" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>856-1060</v>
+      </c>
+      <c r="S13" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="T13" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>8.8512200100000011E-8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
       <c r="B14" s="8">
         <v>476</v>
       </c>
@@ -27536,9 +27713,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="R14" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="S14" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>999-933</v>
+      </c>
+      <c r="T14" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5388402500000001E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
       <c r="B15" s="8">
         <v>269</v>
       </c>
@@ -27593,9 +27782,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+      <c r="R15" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>856-933</v>
+      </c>
+      <c r="S15" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="T15" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>7.7746168899999996E-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="8">
         <v>448</v>
       </c>
@@ -27650,9 +27851,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
+      <c r="R16" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-946</v>
+      </c>
+      <c r="S16" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>959-895</v>
+      </c>
+      <c r="T16" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.8299572840000001E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
       <c r="B17" s="8">
         <v>542</v>
       </c>
@@ -27707,9 +27920,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="R17" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S17" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1041-963</v>
+      </c>
+      <c r="T17" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
       <c r="B18" s="8">
         <v>539</v>
       </c>
@@ -27764,9 +27989,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
+      <c r="R18" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S18" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1057-1010</v>
+      </c>
+      <c r="T18" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
       <c r="B19" s="8">
         <v>272</v>
       </c>
@@ -27821,9 +28058,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="R19" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>856-933</v>
+      </c>
+      <c r="S19" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="T19" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>7.7746168899999996E-8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
       <c r="B20" s="8">
         <v>541</v>
       </c>
@@ -27878,9 +28127,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
+      <c r="R20" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S20" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1069-1041</v>
+      </c>
+      <c r="T20" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
       <c r="B21" s="8">
         <v>353</v>
       </c>
@@ -27935,9 +28196,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="R21" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-955</v>
+      </c>
+      <c r="S21" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="T21" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>7.5078759039999993E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
       <c r="B22" s="8">
         <v>468</v>
       </c>
@@ -27992,9 +28265,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="R22" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="S22" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="T22" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5388402500000001E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="8">
@@ -28049,9 +28334,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+      <c r="R23" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>999-896</v>
+      </c>
+      <c r="S23" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>1060-897</v>
+      </c>
+      <c r="T23" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.0547289999999998E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
       <c r="B24" s="8">
         <v>529</v>
       </c>
@@ -28104,9 +28401,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="R24" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>955-964</v>
+      </c>
+      <c r="S24" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>976-979</v>
+      </c>
+      <c r="T24" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>9.9810090250000007E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
       <c r="B25" s="8">
         <v>467</v>
       </c>
@@ -28159,9 +28468,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+      <c r="R25" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="S25" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T25" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5388402500000001E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
       <c r="B26" s="8">
         <v>446</v>
       </c>
@@ -28214,9 +28535,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="R26" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-946</v>
+      </c>
+      <c r="S26" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T26" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.8299572840000001E-7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
       <c r="B27" s="8">
         <v>444</v>
       </c>
@@ -28269,9 +28602,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+      <c r="R27" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>938-946</v>
+      </c>
+      <c r="S27" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="T27" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.8299572840000001E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
       <c r="B28" s="8">
         <v>377</v>
       </c>
@@ -28324,9 +28669,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+      <c r="R28" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-959</v>
+      </c>
+      <c r="S28" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T28" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3354113599999999E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
       <c r="B29" s="8">
         <v>375</v>
       </c>
@@ -28379,9 +28736,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="R29" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-959</v>
+      </c>
+      <c r="S29" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>938-955</v>
+      </c>
+      <c r="T29" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.3354113599999999E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
       <c r="B30" s="8">
         <v>326</v>
       </c>
@@ -28434,9 +28803,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+      <c r="R30" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-895</v>
+      </c>
+      <c r="S30" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>955-946</v>
+      </c>
+      <c r="T30" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5818092900000001E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
       <c r="B31" s="8">
         <v>324</v>
       </c>
@@ -28489,9 +28870,21 @@
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
+      <c r="R31" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-895</v>
+      </c>
+      <c r="S31" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>933-959</v>
+      </c>
+      <c r="T31" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5818092900000001E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
       <c r="B32" s="8">
         <v>320</v>
       </c>
@@ -28543,6 +28936,18 @@
       <c r="P32" s="10">
         <f>Tabela14[[#This Row],[Q Eq]]+Tabela14[[#This Row],[P Eq]]</f>
         <v>1</v>
+      </c>
+      <c r="R32" s="26" t="str">
+        <f>Tabela14[[#This Row],[De1]]&amp;"-"&amp;Tabela14[[#This Row],[Para1]]</f>
+        <v>933-895</v>
+      </c>
+      <c r="S32" s="26" t="str">
+        <f>Tabela14[[#This Row],[De2]]&amp;"-"&amp;Tabela14[[#This Row],[Para2]]</f>
+        <v>933-959</v>
+      </c>
+      <c r="T32" s="26">
+        <f>Tabela14[[#This Row],[Q Eq]]</f>
+        <v>1.5818092900000001E-6</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>